<commit_message>
data for across incomes, I added clothing and apperals.
</commit_message>
<xml_diff>
--- a/analysis/Data for Income.xlsx
+++ b/analysis/Data for Income.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>Catergories</t>
   </si>
@@ -181,6 +181,30 @@
   </si>
   <si>
     <t>20/1048</t>
+  </si>
+  <si>
+    <t>Apparel and Clothing</t>
+  </si>
+  <si>
+    <t>13/662</t>
+  </si>
+  <si>
+    <t>11/586</t>
+  </si>
+  <si>
+    <t>9/462</t>
+  </si>
+  <si>
+    <t>10/510</t>
+  </si>
+  <si>
+    <t>12/611</t>
+  </si>
+  <si>
+    <t>10/490</t>
+  </si>
+  <si>
+    <t>13/654</t>
   </si>
 </sst>
 </file>
@@ -498,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -680,6 +704,35 @@
         <v>53</v>
       </c>
     </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>